<commit_message>
Add support for more media file types to the application
Expand the list of supported content types to include .heic, .heif, .avi, .webm, .m4a, and .aac to improve media handling.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 9003b42d-cc91-45d4-9bea-08cccc1eb26f
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: a285921b-fd70-422b-9a3b-fb50dc681694
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/2c66ae00-4dc8-48da-a526-15e2ce6c82ec/9003b42d-cc91-45d4-9bea-08cccc1eb26f/fdkS5gO
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/uploads/memories.xlsx
+++ b/uploads/memories.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="ysu+VY8EzKJS+aWjgWK0T2/SL6Q9OJ/Tmpi7k0nrrUs="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="xlB0ReCY1LYWYtd0cCIizI59XiWlcnG++m12rHJjoXg="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="75">
   <si>
     <t>id</t>
   </si>
@@ -42,6 +42,9 @@
     <t>description</t>
   </si>
   <si>
+    <t>tags</t>
+  </si>
+  <si>
     <t>photo_files</t>
   </si>
   <si>
@@ -51,19 +54,67 @@
     <t>audio_files</t>
   </si>
   <si>
+    <t>Dinner at Bistronomy</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>Napier</t>
+  </si>
+  <si>
+    <t>delightful restaurant find when in Napier for Crowded House</t>
+  </si>
+  <si>
+    <t>food</t>
+  </si>
+  <si>
+    <t>FD0101.HEIC, FD0102.HEIC, FD0103.HEIC, FD0104.HEIC, FD0105.HEIC, FD0106.HEIC, FD0107.HEIC</t>
+  </si>
+  <si>
+    <t>Pho at Pho Tung</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
+  </si>
+  <si>
+    <t>Hoi An</t>
+  </si>
+  <si>
+    <t>best pho we've eaten in a wonderful family run restaurant</t>
+  </si>
+  <si>
+    <t>food, travel</t>
+  </si>
+  <si>
+    <t>FD0201.HEIC, FD0202.HEIC, FD0203.HEIC</t>
+  </si>
+  <si>
     <t>Hail at home</t>
   </si>
   <si>
-    <t>New Zealand</t>
-  </si>
-  <si>
     <t>Wellington</t>
   </si>
   <si>
     <t>an unexpected hail storm that passed as swiftly as it arrived</t>
   </si>
   <si>
-    <t>cc624d12-4dfc-4889-8f57-f1c7f34787eb.JPG</t>
+    <t>event</t>
+  </si>
+  <si>
+    <t>EV0101.JPG</t>
+  </si>
+  <si>
+    <t>Ba ba lot</t>
+  </si>
+  <si>
+    <t>Ho Chi Minh</t>
+  </si>
+  <si>
+    <t>favourite food at Quan a co lieng</t>
+  </si>
+  <si>
+    <t>FD0301.PNG</t>
   </si>
   <si>
     <t>Temple adventure</t>
@@ -72,28 +123,124 @@
     <t>Cambodia</t>
   </si>
   <si>
-    <t>Ankor Wat</t>
-  </si>
-  <si>
-    <t>visiting temples</t>
-  </si>
-  <si>
-    <t>IMG_6770.heic</t>
-  </si>
-  <si>
-    <t>Ba ba lot</t>
-  </si>
-  <si>
-    <t>Vietnam</t>
-  </si>
-  <si>
-    <t>Ho Chi Minh</t>
-  </si>
-  <si>
-    <t>favourite food</t>
-  </si>
-  <si>
-    <t>File_015.png</t>
+    <t>Angkor Wat</t>
+  </si>
+  <si>
+    <t>a day visiting temples in and around Angkor Wat</t>
+  </si>
+  <si>
+    <t>travel, event</t>
+  </si>
+  <si>
+    <t>T0101.HEIC, T0102.HEIC, T0103.HEIC, T0104.HEIC, T0105.HEIC, T0106.HEIC, T0107.HEIC, T0108.HEIC, T01009.HEIC, T01010.HEIC, T0111.HEIC, T0112.HEIC</t>
+  </si>
+  <si>
+    <t>Sunrise at home</t>
+  </si>
+  <si>
+    <t>various dates</t>
+  </si>
+  <si>
+    <t>a selection of spectacular sunrises and weather from our home</t>
+  </si>
+  <si>
+    <t>E0201.HEIC, E0202.PNG, E0203.PNG, E0204.HEIC, E0205.HEIC, E0206.HEIC, E0207.HEIC, E0208.HEIC</t>
+  </si>
+  <si>
+    <t>Dinner at Ghost Street</t>
+  </si>
+  <si>
+    <t>Auckland</t>
+  </si>
+  <si>
+    <t>returning to one of our favourite restaurants in Auckland</t>
+  </si>
+  <si>
+    <t>FD0401.HEIC</t>
+  </si>
+  <si>
+    <t>Pluto gig at Double Whammy</t>
+  </si>
+  <si>
+    <t>seeing Dan's favourite Kiwi band reuniting for one night only</t>
+  </si>
+  <si>
+    <t>music</t>
+  </si>
+  <si>
+    <t>M0101.HEIC</t>
+  </si>
+  <si>
+    <t>Day out with the kids</t>
+  </si>
+  <si>
+    <t>spending the day with Cece and Kobe</t>
+  </si>
+  <si>
+    <t>family</t>
+  </si>
+  <si>
+    <t>FA0101.MOV, FA0102.MOV, FA0103.HEIC, FA0104.HEIC, FA0105.HEIC, FA0106.HEIC, FA0107.HEIC, FA0108.HEIC, FA0109.HEIC</t>
+  </si>
+  <si>
+    <t>Crossing Tongariro</t>
+  </si>
+  <si>
+    <t>Tongariro</t>
+  </si>
+  <si>
+    <t>walking the Tongariro crossing together</t>
+  </si>
+  <si>
+    <t>EV0301.HEIC, EV0302.HEIC, EV0303.HEIC, EV0304.HEIC, EV0305.HEIC, EV0306.HEIC, EV0307.HEIC, EV0308.HEIC, EV0309.HEIC, EV0310.HEIC, EV0311.HEIC, EV0312.HEIC, EV0313.HEIC, EV0314.HEIC, EV0315.HEIC, EV0316.HEIC, EV0317.HEIC, EV0318.HEIC, EV0319.HEIC, EV0320.HEIC, EV0321.HEIC</t>
+  </si>
+  <si>
+    <t>Dad's 70th in Karkoura</t>
+  </si>
+  <si>
+    <t>Kaikoura</t>
+  </si>
+  <si>
+    <t>spending a weekend in Kaikoura for Dan's Dad's 70th birthday</t>
+  </si>
+  <si>
+    <t>family, event</t>
+  </si>
+  <si>
+    <t>FA0201.HEIC, FA0202.HEIC, FA0203.HEIC, FA0204.HEIC</t>
+  </si>
+  <si>
+    <t>Our engagement</t>
+  </si>
+  <si>
+    <t>photos of our engagement and the engagement ring</t>
+  </si>
+  <si>
+    <t>EV0401.HEIC, EV0402.HEIC, EV0403.HEIC, EV0404.JPG, EV0405.JPG, EV0406.JPG, EV0407.JPG, EV0408.HEIC, EV0409.MOV</t>
+  </si>
+  <si>
+    <t>Seeing Michael in Hong Kong</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>having cocktails with Michael at Iron Fairies in Hong Kong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">travel </t>
+  </si>
+  <si>
+    <t>T0201.HEIC</t>
+  </si>
+  <si>
+    <t>Soti in Wellington</t>
+  </si>
+  <si>
+    <t>catching up with Soti at Pickle and Pie</t>
+  </si>
+  <si>
+    <t>FA0301.HEIC</t>
   </si>
 </sst>
 </file>
@@ -103,7 +250,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yy"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -114,6 +261,11 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -130,19 +282,28 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
@@ -359,6 +520,19 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="3.0"/>
+    <col customWidth="1" min="2" max="2" width="13.56"/>
+    <col customWidth="1" min="3" max="3" width="10.22"/>
+    <col customWidth="1" min="4" max="4" width="8.67"/>
+    <col customWidth="1" min="5" max="5" width="7.33"/>
+    <col customWidth="1" min="6" max="7" width="12.78"/>
+    <col customWidth="1" min="8" max="8" width="25.44"/>
+    <col customWidth="1" min="9" max="9" width="10.22"/>
+    <col customWidth="1" min="10" max="10" width="17.44"/>
+    <col customWidth="1" min="11" max="11" width="9.44"/>
+    <col customWidth="1" min="12" max="12" width="8.78"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -394,92 +568,456 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>1.0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="3">
-        <v>-41.2954799654563</v>
-      </c>
-      <c r="F2" s="3">
-        <v>174.799988654323</v>
-      </c>
-      <c r="G2" s="4">
-        <v>45958.0</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="E2" s="4">
+        <v>-39.4889855933606</v>
+      </c>
+      <c r="F2" s="4">
+        <v>176.918171525006</v>
+      </c>
+      <c r="G2" s="5">
+        <v>44276.0</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>15</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1">
+      <c r="A3" s="6">
         <v>2.0</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="B3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="2">
-        <v>13.4126780110813</v>
-      </c>
-      <c r="F3" s="2">
-        <v>103.866974967744</v>
+      <c r="C3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="6">
+        <v>15.8777112018275</v>
+      </c>
+      <c r="F3" s="6">
+        <v>108.328979895228</v>
       </c>
       <c r="G3" s="5">
-        <v>45859.0</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>20</v>
+        <v>45828.0</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1">
+      <c r="A4" s="6">
         <v>3.0</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="2">
+        <v>-41.2954799654563</v>
+      </c>
+      <c r="F4" s="7">
+        <v>174.7999885</v>
+      </c>
+      <c r="G4" s="5">
+        <v>45958.0</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6">
+        <v>4.0</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="2">
+        <v>10.7716922873018</v>
+      </c>
+      <c r="F5" s="2">
+        <v>106.68578776771</v>
+      </c>
+      <c r="G5" s="5">
+        <v>45860.0</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="2">
-        <v>10.7716922873018</v>
-      </c>
-      <c r="F4" s="2">
-        <v>106.68578776771</v>
-      </c>
-      <c r="G4" s="5">
+      <c r="J5" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="2">
+        <v>13.4126780110813</v>
+      </c>
+      <c r="F6" s="2">
+        <v>103.866974967744</v>
+      </c>
+      <c r="G6" s="5">
+        <v>45859.0</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="2">
+        <v>-41.2954799654563</v>
+      </c>
+      <c r="F7" s="7">
+        <v>174.7999886</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="6">
+        <v>-36.8446415107819</v>
+      </c>
+      <c r="F8" s="6">
+        <v>174.768587611373</v>
+      </c>
+      <c r="G8" s="8">
+        <v>45969.0</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6">
+        <v>8.0</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="6">
+        <v>-36.8573162559551</v>
+      </c>
+      <c r="F9" s="6">
+        <v>174.760031307669</v>
+      </c>
+      <c r="G9" s="8">
+        <v>45969.0</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6">
+        <v>9.0</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="6">
+        <v>-41.2889316739713</v>
+      </c>
+      <c r="F10" s="6">
+        <v>174.800056887522</v>
+      </c>
+      <c r="G10" s="8">
+        <v>45955.0</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6">
+        <v>10.0</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="6">
+        <v>-39.1337067069664</v>
+      </c>
+      <c r="F11" s="6">
+        <v>175.655977735188</v>
+      </c>
+      <c r="G11" s="8">
+        <v>44674.0</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6">
+        <v>11.0</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="6">
+        <v>-42.400718306509</v>
+      </c>
+      <c r="F12" s="6">
+        <v>173.681216323288</v>
+      </c>
+      <c r="G12" s="8">
+        <v>44940.0</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6">
+        <v>12.0</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="2">
+        <v>-41.2954799654563</v>
+      </c>
+      <c r="F13" s="7">
+        <v>174.7999887</v>
+      </c>
+      <c r="G13" s="8">
+        <v>45808.0</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6">
+        <v>13.0</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="6">
+        <v>22.282069528999</v>
+      </c>
+      <c r="F14" s="6">
+        <v>114.154705499113</v>
+      </c>
+      <c r="G14" s="8">
         <v>45860.0</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="2" t="s">
+      <c r="H14" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6">
+        <v>14.0</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>25</v>
+      </c>
+      <c r="E15" s="6">
+        <v>-41.2896477452698</v>
+      </c>
+      <c r="F15" s="6">
+        <v>174.776203747817</v>
+      </c>
+      <c r="G15" s="8">
+        <v>45865.0</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Update memory card bottom padding to match user request
Adjust the bottom padding of memory detail cards in MemoryDetail.tsx from pb-12 to pb-20 to increase the bottom border size as requested.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 9003b42d-cc91-45d4-9bea-08cccc1eb26f
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 3b9ca9a7-8c4f-496b-851d-881ab2f758a0
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/2c66ae00-4dc8-48da-a526-15e2ce6c82ec/9003b42d-cc91-45d4-9bea-08cccc1eb26f/4pMjFaR
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/uploads/memories.xlsx
+++ b/uploads/memories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="91">
   <si>
     <t>id</t>
   </si>
@@ -144,7 +144,7 @@
     <t>a selection of spectacular sunrises and weather from our home</t>
   </si>
   <si>
-    <t>E0201.HEIC, E0202.PNG, E0203.PNG, E0204.HEIC, E0205.HEIC, E0206.HEIC, E0207.HEIC, E0208.HEIC</t>
+    <t>EV0201.HEIC, EV0202.PNG, EV0203.PNG, EV0204.HEIC, EV0205.HEIC, EV0206.HEIC, EV0207.HEIC, EV0208.HEIC</t>
   </si>
   <si>
     <t>Dinner at Ghost Street</t>
@@ -180,7 +180,7 @@
     <t>family</t>
   </si>
   <si>
-    <t>FA0101.MOV, FA0102.MOV, FA0103.HEIC, FA0104.HEIC, FA0105.HEIC, FA0106.HEIC, FA0107.HEIC, FA0108.HEIC, FA0109.HEIC</t>
+    <t>FA0101.MOV, FA0102.MOV, FA0103.HEIC, FA0104.HEIC, FA0106.HEIC, FA0107.HEIC, FA0109.HEIC</t>
   </si>
   <si>
     <t>Crossing Tongariro</t>
@@ -241,14 +241,63 @@
   </si>
   <si>
     <t>FA0301.HEIC</t>
+  </si>
+  <si>
+    <t>Blue Duck Station</t>
+  </si>
+  <si>
+    <t>Whanganui National Park</t>
+  </si>
+  <si>
+    <t>a surprise trip booked by Alex, to a spectacular and picturesque location</t>
+  </si>
+  <si>
+    <t>EV0501.JPEG, EV0502.JPEG, EV0503.JPEG, EV0504.JPEG, EV0505.JPEG, EV0506.JPEG, EV0507.JPEG, EV0508.JPEG, EV0509.JPEG, EV0510.JPEG, EV0511.JPEG, EV0512.JPEG, EV0513.JPEG, EV0514.JPEG, EV0515.JPEG, EV0516.JPEG</t>
+  </si>
+  <si>
+    <t>Chefs Table</t>
+  </si>
+  <si>
+    <t>on top of the world, sharing the best meal we've had</t>
+  </si>
+  <si>
+    <t>FD0501.JPEG, FD0502.JPEG, FD0503.JPEG, FD0504.JPEG, FD0505.JPEG, FD0506.JPEG, FD0507.JPEG, FD0508.JPEG, FD0509.JPEG, FD0510.JPEG, FD0511.JPEG, FD0512.JPEG, FD0513.JPEG, FD0514.JPEG, FD0515.JPEG, FD0516.JPEG, FD0517.JPEG, FD0518.JPEG, FD0519.JPEG</t>
+  </si>
+  <si>
+    <t>Sydney visit</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>catching up with friends in Sydney</t>
+  </si>
+  <si>
+    <t>travel</t>
+  </si>
+  <si>
+    <t>T0301.JPEG, T0302.JPEG, T0303.JPEG, T0304.JPEG, T0305.JPEG</t>
+  </si>
+  <si>
+    <t>Quay restaurant</t>
+  </si>
+  <si>
+    <t>a Michelin starred meal for Alex's birthday</t>
+  </si>
+  <si>
+    <t>FD0601.JPEG, FD0602.JPEG, FD0603.JPEG, FD0604.JPEG, FD0605.JPEG, FD0606.JPEG, FD0607.JPEG, FD0608.JPEG, FD0609.JPEG, FD0610.JPEG, FD0611.JPEG, FD06012JPEG, FD0613.JPEG, FD0614.JPEG, FD0615.JPEG, FD0616.JPEG, FD0617.JPEG, FD0618.JPEG, FD0619.JPEG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d/m/yy"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -282,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -306,6 +355,9 @@
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1018,6 +1070,134 @@
       </c>
       <c r="J15" s="6" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6">
+        <v>15.0</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="6">
+        <v>-39.1060708640499</v>
+      </c>
+      <c r="F16" s="6">
+        <v>175.072770580047</v>
+      </c>
+      <c r="G16" s="8">
+        <v>45438.0</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6">
+        <v>16.0</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="6">
+        <v>-39.1371237525731</v>
+      </c>
+      <c r="F17" s="6">
+        <v>175.063410264329</v>
+      </c>
+      <c r="G17" s="8">
+        <v>45438.0</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="6">
+        <v>17.0</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="6">
+        <v>-33.8776089326146</v>
+      </c>
+      <c r="F18" s="6">
+        <v>151.103222553193</v>
+      </c>
+      <c r="G18" s="8">
+        <v>45368.0</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6">
+        <v>18.0</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" s="6">
+        <v>-33.8574350305951</v>
+      </c>
+      <c r="F19" s="6">
+        <v>151.210148768535</v>
+      </c>
+      <c r="G19" s="9">
+        <v>45367.0</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>